<commit_message>
Added test for verification of broken links on html and exporting to excel
</commit_message>
<xml_diff>
--- a/src/main/resources/data/login.xlsx
+++ b/src/main/resources/data/login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shali\OneDrive\Documents\Resume\Interview prep\seleniumPracticeCodes\webAutomationFramework\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F439660-FDD4-4431-8434-980DB4BB3EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E6DA5-510A-49F0-A177-280DBACD8F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1440" windowWidth="14400" windowHeight="7270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>

</xml_diff>